<commit_message>
test local commit hook
</commit_message>
<xml_diff>
--- a/sheet/TrinketCardData.xlsx
+++ b/sheet/TrinketCardData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\datasheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7E9AC9-2E5B-4E9C-ADAA-A7C3B7312170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28FA2F4-67A3-4A10-8103-DE4B6EBCE7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>cardName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -197,6 +197,10 @@
   </si>
   <si>
     <t>选弃牌堆1张牌放在房间区任意非空列任意位置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DD pocket</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -249,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -258,6 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -541,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -693,6 +698,9 @@
       <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="C11" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
test local commit hook 2
</commit_message>
<xml_diff>
--- a/sheet/TrinketCardData.xlsx
+++ b/sheet/TrinketCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28FA2F4-67A3-4A10-8103-DE4B6EBCE7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8235F4-7747-4C61-B8A2-2BC30C3EC8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,15 +192,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>选弃牌堆1张牌放在房间区任意非空列任意位置。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>DD pocket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -253,7 +253,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -262,7 +262,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -546,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -612,7 +611,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>24</v>
@@ -696,10 +695,10 @@
         <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="4" t="s">
         <v>41</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test local commit hook 3
</commit_message>
<xml_diff>
--- a/sheet/TrinketCardData.xlsx
+++ b/sheet/TrinketCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8235F4-7747-4C61-B8A2-2BC30C3EC8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEC437D-0446-4E3E-8631-7E10519E456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。Test</t>
+    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
test local commit hook 4
</commit_message>
<xml_diff>
--- a/sheet/TrinketCardData.xlsx
+++ b/sheet/TrinketCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEC437D-0446-4E3E-8631-7E10519E456A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879BFC69-F595-4B64-B58B-C9511A1FF734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。</t>
+    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +546,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
test local commit hook 5
</commit_message>
<xml_diff>
--- a/sheet/TrinketCardData.xlsx
+++ b/sheet/TrinketCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879BFC69-F595-4B64-B58B-C9511A1FF734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F938DA-EF9C-4181-8533-88287D75550F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。Test</t>
+    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +546,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
test local commit hook 6
</commit_message>
<xml_diff>
--- a/sheet/TrinketCardData.xlsx
+++ b/sheet/TrinketCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F938DA-EF9C-4181-8533-88287D75550F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE2B006-2F81-46D5-B833-20EDFDBCF9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。</t>
+    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +546,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Test local commit hook done. Reset.
</commit_message>
<xml_diff>
--- a/sheet/TrinketCardData.xlsx
+++ b/sheet/TrinketCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE2B006-2F81-46D5-B833-20EDFDBCF9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E11C0F-E1A0-4D1A-A197-A85245B4056D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,7 +200,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。Test</t>
+    <t>空档区有空位时可以发动：将1张手牌放入空档区，然后抽2张牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +546,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>